<commit_message>
add Recording entity,add Policy entity
</commit_message>
<xml_diff>
--- a/Document/项目的需求分析/软件设计.xlsx
+++ b/Document/项目的需求分析/软件设计.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="111">
   <si>
     <t>规则</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -77,14 +77,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>策略变更时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>datatime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>策略理由</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -295,10 +287,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>所属老师</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>用户微信</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -346,15 +334,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;Recording&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Team</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>changeTime</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -453,10 +433,6 @@
   </si>
   <si>
     <t>团队表设计Team</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userInfo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -526,10 +502,6 @@
   </si>
   <si>
     <t>所属策略</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>policy</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -624,8 +596,110 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>记录表设计Recording</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>策略表设计Policy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>记录人员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RecordingType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">1:1 </t>
+      <t xml:space="preserve">N:1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>关联用户表</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>团队队长</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>leader</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>团队成员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;User&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>recordingTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>团队简介</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>团队口号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>slogan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>policy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>recorder</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">N:N </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>关联用户表</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">N:1 </t>
     </r>
     <r>
       <rPr>
@@ -650,37 +724,25 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>记录表设计Recording</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>策略表设计Policy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>记录人员</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RecordPersonnel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RecordingType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">N:1 </t>
-    </r>
+    <t>Float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所属老师</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>creator</t>
+  </si>
+  <si>
+    <t>Recording</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -689,71 +751,18 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>关联用户表</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>团队队长</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>leader</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>团队成员</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;User&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1:N </t>
+      <t>关系名</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>关联用户表</t>
+      <t>policy</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>policyType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>policyStatus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>recordingTime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>团队简介</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>团队口号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>slogan</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -815,7 +824,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -825,12 +834,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -853,7 +856,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -915,26 +918,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5448,10 +5439,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5460,27 +5451,27 @@
     <col min="2" max="2" width="18.625" style="16" customWidth="1"/>
     <col min="3" max="4" width="18.625" style="2" customWidth="1"/>
     <col min="5" max="5" width="18.625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="34.125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="60" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="24.95" customHeight="1">
-      <c r="B1" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7" s="6" customFormat="1" ht="38.1" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>0</v>
@@ -5488,7 +5479,7 @@
       <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5497,10 +5488,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>4</v>
@@ -5512,19 +5503,19 @@
         <v>5</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>54</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="G4" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1">
@@ -5532,16 +5523,16 @@
         <v>7</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="G5" t="s">
-        <v>107</v>
+      <c r="F5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1">
@@ -5552,537 +5543,535 @@
         <v>106</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G6" t="s">
-        <v>107</v>
+        <v>52</v>
+      </c>
+      <c r="F6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1">
-      <c r="A7" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="21"/>
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" ht="18" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F8" s="14"/>
-      <c r="G8" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="18" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>82</v>
+        <v>105</v>
+      </c>
+      <c r="F10" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G11" t="s">
-        <v>107</v>
+        <v>76</v>
+      </c>
+      <c r="F11" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G12" t="s">
-        <v>107</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="18" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="18" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18" customHeight="1">
-      <c r="A16" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>83</v>
+      <c r="A16" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="19"/>
+      <c r="E16" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="18" customHeight="1">
-      <c r="A17" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="24" t="s">
+      <c r="A17" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17" t="s">
-        <v>107</v>
+      <c r="D17" s="19"/>
+      <c r="E17" s="20" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="18" customHeight="1">
-      <c r="A18" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" t="s">
-        <v>107</v>
+      <c r="A18" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="18" customHeight="1">
-      <c r="A19" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" t="s">
-        <v>107</v>
-      </c>
+      <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:7" ht="18" customHeight="1">
-      <c r="A20" s="1"/>
-    </row>
+    <row r="20" spans="1:7" ht="18" customHeight="1"/>
     <row r="21" spans="1:7" ht="18" customHeight="1"/>
     <row r="22" spans="1:7" ht="18" customHeight="1"/>
     <row r="23" spans="1:7" ht="18" customHeight="1"/>
-    <row r="24" spans="1:7" ht="18" customHeight="1"/>
-    <row r="25" spans="1:7" s="3" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A25" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="10"/>
+    <row r="24" spans="1:7" s="3" customFormat="1" ht="24.95" customHeight="1">
+      <c r="A24" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="G24" s="10"/>
     </row>
-    <row r="26" spans="1:7" s="6" customFormat="1" ht="38.1" customHeight="1">
-      <c r="A26" s="4" t="s">
+    <row r="25" spans="1:7" s="6" customFormat="1" ht="38.1" customHeight="1">
+      <c r="A25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="18" customHeight="1">
+      <c r="A26" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>21</v>
-      </c>
+      <c r="B26" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="9"/>
     </row>
     <row r="27" spans="1:7" ht="18" customHeight="1">
-      <c r="A27" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="9"/>
+      <c r="A27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" t="s">
+        <v>95</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="18" customHeight="1">
-      <c r="A28" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="B28" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="C28" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="D28" s="24"/>
-      <c r="E28" s="25" t="s">
-        <v>99</v>
-      </c>
+      <c r="A28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="1:7" ht="18" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>90</v>
+        <v>75</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="F29" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18" customHeight="1">
-      <c r="A30" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="F30" s="13"/>
+      <c r="A30" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" s="19"/>
+      <c r="E30" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F30" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="18" customHeight="1">
-      <c r="A31" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" s="1"/>
+      <c r="A31" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="18" customHeight="1">
-      <c r="A32" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="D32" s="19"/>
-      <c r="E32" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="F32" s="21"/>
+      <c r="A32" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
     </row>
-    <row r="33" spans="1:7" ht="18" customHeight="1">
-      <c r="A33" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
+    <row r="33" spans="1:7" s="6" customFormat="1" ht="38.1" customHeight="1">
+      <c r="A33" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G33" s="11"/>
     </row>
-    <row r="34" spans="1:7" s="6" customFormat="1" ht="38.1" customHeight="1">
-      <c r="A34" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F34" s="11"/>
+    <row r="34" spans="1:7" ht="18" customHeight="1">
+      <c r="A34" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="9"/>
     </row>
     <row r="35" spans="1:7" ht="18" customHeight="1">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E35" s="9"/>
+      <c r="B35" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="F35" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="18" customHeight="1">
-      <c r="A36" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="B36" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="C36" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="D36" s="24"/>
-      <c r="E36" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" t="s">
-        <v>107</v>
-      </c>
+      <c r="A36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="1"/>
     </row>
     <row r="37" spans="1:7" ht="18" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D37" s="1"/>
-      <c r="G37" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="38" spans="1:7" ht="18" customHeight="1">
-      <c r="A38" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38" s="1"/>
+      <c r="A38" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="19"/>
+      <c r="E38" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="18" customHeight="1">
-      <c r="A39" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="1"/>
+      <c r="A39" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="D39" s="19"/>
+      <c r="E39" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="F39" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="18" customHeight="1">
-      <c r="A40" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="B40" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="D40" s="24"/>
-      <c r="E40" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="G40" t="s">
-        <v>107</v>
-      </c>
+      <c r="A40" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
     </row>
-    <row r="41" spans="1:7" ht="18" customHeight="1">
-      <c r="A41" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
+    <row r="41" spans="1:7" s="6" customFormat="1" ht="38.1" customHeight="1">
+      <c r="A41" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G41" s="11"/>
     </row>
-    <row r="42" spans="1:7" s="6" customFormat="1" ht="38.1" customHeight="1">
-      <c r="A42" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F42" s="11"/>
+    <row r="42" spans="1:7" ht="18" customHeight="1">
+      <c r="A42" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="9"/>
     </row>
     <row r="43" spans="1:7" ht="18" customHeight="1">
-      <c r="A43" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E43" s="9"/>
+      <c r="A43" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" s="1"/>
     </row>
     <row r="44" spans="1:7" ht="18" customHeight="1">
       <c r="A44" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D44" s="1"/>
     </row>
     <row r="45" spans="1:7" ht="18" customHeight="1">
-      <c r="A45" s="2" t="s">
-        <v>37</v>
+      <c r="A45" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:7" ht="18" customHeight="1">
-      <c r="A46" s="1" t="s">
-        <v>39</v>
+      <c r="A46" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:7" ht="18" customHeight="1">
-      <c r="A47" s="2" t="s">
-        <v>41</v>
+      <c r="A47" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D47" s="1"/>
     </row>
     <row r="48" spans="1:7" ht="18" customHeight="1">
-      <c r="A48" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B48" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="D48" s="1"/>
     </row>
     <row r="49" spans="4:4" ht="18" customHeight="1">
@@ -6112,15 +6101,12 @@
     <row r="57" spans="4:4" ht="18" customHeight="1">
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="4:4" ht="18" customHeight="1">
-      <c r="D58" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A40:E40"/>
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A24:E24"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>